<commit_message>
added validation and refactored script
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_mitb\nlp_assignment2\bert_sentiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F942DC34-E7E3-4145-92DE-20D7DEDB2EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3133CBAD-EFB2-4F3F-B745-0CADEFF502E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23184" yWindow="1872" windowWidth="15672" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16332" yWindow="2088" windowWidth="22176" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Model</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Config</t>
-  </si>
-  <si>
-    <t>Best Accuracy</t>
   </si>
   <si>
     <t>lowercase</t>
@@ -76,6 +73,20 @@
 epochs = 5
 use_gpu_predict = False
 lr = 1e-5</t>
+  </si>
+  <si>
+    <t>Best Accuracy (Val-Split)</t>
+  </si>
+  <si>
+    <t>Best Accuracy (Val-Excel)</t>
+  </si>
+  <si>
+    <t>Best Accuracy (Val-Excel) uses test size of 0.00001</t>
+  </si>
+  <si>
+    <t>accuracy    precision-neg    recall-neg    f1-neg
+----------  ---------------  ------------  --------
+86.95%      85.55%           88.89%        87.19%</t>
   </si>
 </sst>
 </file>
@@ -117,12 +128,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -415,10 +429,12 @@
     <col min="2" max="2" width="15.109375" customWidth="1"/>
     <col min="3" max="3" width="26.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.33203125" customWidth="1"/>
+    <col min="7" max="7" width="43.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,16 +442,22 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -443,7 +465,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -452,15 +474,15 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
@@ -469,15 +491,15 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
@@ -486,15 +508,15 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
@@ -503,24 +525,27 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D7" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added latest results of experiments
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_mitb\nlp_assignment2\bert_sentiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE6592F-D9DE-4A6D-8144-43804C8853ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CD79B2-9542-4CD4-A2EC-E7B6C12F052F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17820" yWindow="1596" windowWidth="20232" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19212" yWindow="2988" windowWidth="20232" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>Model</t>
   </si>
@@ -104,6 +104,26 @@
     <t>accuracy    f1_macro    precision-neg    recall-neg
 ----------  ----------  ---------------  ------------
 92.6%       92.6%       93.29%           91.79%</t>
+  </si>
+  <si>
+    <t>accuracy    f1_macro    precision-neg    recall-neg
+----------  ----------  ---------------  ------------
+88.05%      88.05%      87.62%           88.59%</t>
+  </si>
+  <si>
+    <t>lowercase
+truncate 382/128 split</t>
+  </si>
+  <si>
+    <t>seed = 1234
+test_size = 0.2
+MAX_LEN = 512
+START_LEN = 382
+END_LEN = 128
+batch_size = 16
+epochs = 10
+use_gpu_test = True
+lr = 1e-5</t>
   </si>
 </sst>
 </file>
@@ -435,16 +455,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
     <col min="4" max="4" width="26.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.77734375" bestFit="1" customWidth="1"/>
@@ -604,6 +625,29 @@
         <v>18</v>
       </c>
     </row>
+    <row r="8" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8">
+        <v>0.9</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
run bert large experiment
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_mitb\nlp_assignment2\bert_sentiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CD79B2-9542-4CD4-A2EC-E7B6C12F052F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436B92BF-C17B-485D-B551-AD6BE36D58B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19212" yWindow="2988" windowWidth="20232" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,7 +467,7 @@
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5546875" customWidth="1"/>
     <col min="4" max="4" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" customWidth="1"/>
     <col min="6" max="6" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.33203125" customWidth="1"/>
     <col min="8" max="8" width="43.5546875" customWidth="1"/>

</xml_diff>

<commit_message>
refactored and try change dropout rate
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_mitb\nlp_assignment2\bert_sentiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436B92BF-C17B-485D-B551-AD6BE36D58B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F53238-E766-49A9-8599-0F64F7A8D4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19212" yWindow="2988" windowWidth="20232" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Model</t>
   </si>
@@ -124,6 +124,23 @@
 epochs = 10
 use_gpu_test = True
 lr = 1e-5</t>
+  </si>
+  <si>
+    <t>bert-base-cased</t>
+  </si>
+  <si>
+    <t>seed = 1234
+test_size = 0.2
+MAX_LEN = 512
+batch_size = 16
+epochs = 10
+use_gpu_predict = False
+lr = 1e-5</t>
+  </si>
+  <si>
+    <t>accuracy    f1_macro    precision-neg    recall-neg
+----------  ----------  ---------------  ------------
+91.65%      91.65%      89.69%           94.09%</t>
   </si>
 </sst>
 </file>
@@ -455,11 +472,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,6 +665,29 @@
         <v>19</v>
       </c>
     </row>
+    <row r="9" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9">
+        <v>0.94</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated test and validation scripts
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_mitb\nlp_assignment2\bert_sentiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F53238-E766-49A9-8599-0F64F7A8D4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D3E6F3-5EB8-4DCC-9838-530D08B3B00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Model</t>
   </si>
@@ -99,11 +99,6 @@
   </si>
   <si>
     <t>Id</t>
-  </si>
-  <si>
-    <t>accuracy    f1_macro    precision-neg    recall-neg
-----------  ----------  ---------------  ------------
-92.6%       92.6%       93.29%           91.79%</t>
   </si>
   <si>
     <t>accuracy    f1_macro    precision-neg    recall-neg
@@ -156,18 +151,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -182,12 +171,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -476,7 +464,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,10 +600,10 @@
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>0.88</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -635,12 +623,10 @@
       <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="F7" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -650,19 +636,19 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="F8">
         <v>0.9</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -670,22 +656,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="F9">
         <v>0.94</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update model to uncased
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_mitb\nlp_assignment2\bert_sentiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D3E6F3-5EB8-4DCC-9838-530D08B3B00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B496577F-C079-4338-B7B5-7B776EAE4F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>Model</t>
   </si>
@@ -136,6 +136,24 @@
     <t>accuracy    f1_macro    precision-neg    recall-neg
 ----------  ----------  ---------------  ------------
 91.65%      91.65%      89.69%           94.09%</t>
+  </si>
+  <si>
+    <t>accuracy    f1_macro    precision-neg    recall-neg
+----------  ----------  ---------------  ------------
+91.1%       91.1%       90.05%           92.39%</t>
+  </si>
+  <si>
+    <t>seed = 1234
+test_size = 0.2
+MAX_LEN = 512
+START_LEN = 382
+END_LEN = 128
+batch_size = 16
+epochs = 7
+ATTENTION_PROB_DROPOUT_PROB=0.2
+HIDDEN_DROPOUT_PROB=0.2
+SAVE_PROCESSED = True
+use_gpu_test = True</t>
   </si>
 </sst>
 </file>
@@ -151,12 +169,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -171,11 +195,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -460,11 +485,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,7 +497,7 @@
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5546875" customWidth="1"/>
     <col min="4" max="4" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.77734375" customWidth="1"/>
+    <col min="5" max="5" width="39.33203125" customWidth="1"/>
     <col min="6" max="6" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.33203125" customWidth="1"/>
     <col min="8" max="8" width="43.5546875" customWidth="1"/>
@@ -600,10 +625,10 @@
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="4">
         <v>0.88</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -623,10 +648,12 @@
       <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="4">
         <v>0.93</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -667,11 +694,28 @@
       <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>0.94</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>